<commit_message>
Add weigthed adjacency matrix
</commit_message>
<xml_diff>
--- a/AdjMatrix.xlsx
+++ b/AdjMatrix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Temp\adjmat2graph\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F123268B-531B-4DBF-BF77-6BB2BFD651D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573EF019-7D46-4A22-AA11-097403CA3085}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="315" yWindow="825" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matrix" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>Simon</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Franzi</t>
+  </si>
+  <si>
+    <t>Horst</t>
   </si>
 </sst>
 </file>
@@ -375,15 +378,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -411,14 +414,14 @@
       <c r="J1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
       <c r="C2">
         <v>1</v>
       </c>
@@ -426,7 +429,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -438,21 +441,21 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -467,27 +470,27 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
       <c r="E4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -498,14 +501,14 @@
       <c r="J4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
       <c r="F5">
         <v>1</v>
       </c>
@@ -513,7 +516,7 @@
         <v>1</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -521,14 +524,14 @@
       <c r="J5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
       <c r="G6">
         <v>0</v>
       </c>
@@ -536,19 +539,19 @@
         <v>1</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
       <c r="H7">
         <v>1</v>
       </c>
@@ -558,38 +561,46 @@
       <c r="J7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
       <c r="I8">
         <v>1</v>
       </c>
       <c r="J8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
       <c r="J9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="J10">
-        <v>0</v>
+      <c r="K10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>